<commit_message>
Update Report CP & Add Cp Evaluation
</commit_message>
<xml_diff>
--- a/includes/file_modele/template-cp-evaluation.xlsx
+++ b/includes/file_modele/template-cp-evaluation.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25629"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\stage\wp-content\plugins\orion-task-manager\includes\file_modele\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\oriontest\wp-content\plugins\orion-task-manager\includes\file_modele\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D36E4F00-3521-4C23-B7A0-F36ACEDF933E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{683A0630-5D00-4ACF-8DA2-07F5BA0CC3CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CP_RAPPORT" sheetId="1" r:id="rId1"/>
+    <sheet name="EVALUATION" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -30,25 +31,124 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
   <si>
     <t>N°</t>
   </si>
   <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t>List Of Goals</t>
-  </si>
-  <si>
-    <t>Project Managers</t>
+    <t>NUMBER OF TASKS COMPLETED:</t>
+  </si>
+  <si>
+    <t>NOTE</t>
+  </si>
+  <si>
+    <t>Completed</t>
+  </si>
+  <si>
+    <t>Work Quality</t>
+  </si>
+  <si>
+    <t>Deadline</t>
+  </si>
+  <si>
+    <t>Commit</t>
+  </si>
+  <si>
+    <t>Collaboration</t>
+  </si>
+  <si>
+    <t>Work consistency</t>
+  </si>
+  <si>
+    <t>Full Name</t>
+  </si>
+  <si>
+    <t>Month</t>
+  </si>
+  <si>
+    <t>HOW WORK WAS DONE?</t>
+  </si>
+  <si>
+    <t>Goals</t>
+  </si>
+  <si>
+    <t>ORION ORIGIN REPORT PROJECT MANAGER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MONTH : </t>
+  </si>
+  <si>
+    <t>EMPLOYEE NAME</t>
+  </si>
+  <si>
+    <t>DEPARTMENT</t>
+  </si>
+  <si>
+    <t>POSITION HELD</t>
+  </si>
+  <si>
+    <t>CHARACTERISTICS</t>
+  </si>
+  <si>
+    <t>WHAT WORK WAS DONE?</t>
+  </si>
+  <si>
+    <t>UNSATISFACTORY (0 - 39)</t>
+  </si>
+  <si>
+    <t>FAIR (40 - 60)</t>
+  </si>
+  <si>
+    <t>GOOD (61 - 85)</t>
+  </si>
+  <si>
+    <t>EXCELLENT (86 - 100)</t>
+  </si>
+  <si>
+    <t>General Performance: Goals versus Accomplishment</t>
+  </si>
+  <si>
+    <t>Overall rating from Support Department</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Initiative &amp; Creativity: Ability to understand, plan work, and to proceed with a task without being told every detail + the ability to make constructive suggestions)</t>
+  </si>
+  <si>
+    <t>Additional Projects: Custom Jobs</t>
+  </si>
+  <si>
+    <t>TEAM MEMBER WORK LOG</t>
+  </si>
+  <si>
+    <t>ROUND-UP OF WORK DONE SINCE PREVIOUS PERORMANCE REVIEW</t>
+  </si>
+  <si>
+    <t>MOVING FORWARD</t>
+  </si>
+  <si>
+    <t>TOP STRENGTH(S)</t>
+  </si>
+  <si>
+    <t>GROWTH AREA(S)</t>
+  </si>
+  <si>
+    <t>ADDITIONAL COMMENTS</t>
+  </si>
+  <si>
+    <t>PROJECT MANAGER</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
+  </numFmts>
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -56,20 +156,63 @@
     </font>
     <font>
       <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Roboto"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Roboto"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Roboto"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <color theme="1"/>
+      <name val="Roboto"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
       <b/>
-      <sz val="16"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Roboto"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Roboto"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Roboto"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Roboto"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -78,12 +221,54 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor rgb="FFF3F3F3"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor rgb="FFF3F3F3"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor rgb="FFF3F3F3"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF009AB2"/>
+        <bgColor rgb="FF009AB2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA4C7CC"/>
+        <bgColor rgb="FFA4C7CC"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -106,18 +291,430 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="9" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -423,54 +1020,429 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="7" style="1" customWidth="1"/>
-    <col min="3" max="3" width="129.5703125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="23.140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="5.140625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="32" style="3" customWidth="1"/>
+    <col min="4" max="4" width="61.85546875" style="3" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" style="3" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="12" style="3" customWidth="1"/>
+    <col min="9" max="9" width="11.5703125" style="3" customWidth="1"/>
+    <col min="10" max="10" width="16" style="3" customWidth="1"/>
+    <col min="11" max="11" width="19.28515625" style="3" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="28"/>
+    </row>
+    <row r="2" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2"/>
+      <c r="B2" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="8"/>
+      <c r="F2" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="25"/>
+      <c r="K2" s="8"/>
+    </row>
+    <row r="3" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2"/>
+      <c r="B3" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="21"/>
+      <c r="E3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G3" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="K3" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="22"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="4"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="4"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="4"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <mergeCells count="4">
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="F2:J2"/>
+    <mergeCell ref="D1:K1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4E09C5B-1631-4BD2-B25A-755DF0E42D08}">
+  <dimension ref="A1:G27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:G4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2.85546875" customWidth="1"/>
+    <col min="2" max="2" width="48.42578125" customWidth="1"/>
+    <col min="4" max="4" width="38.28515625" customWidth="1"/>
+    <col min="5" max="5" width="21.28515625" customWidth="1"/>
+    <col min="6" max="6" width="20.140625" customWidth="1"/>
+    <col min="7" max="7" width="23.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="9"/>
+      <c r="B1" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="63"/>
+      <c r="D1" s="64"/>
+      <c r="E1" s="64"/>
+      <c r="F1" s="64"/>
+      <c r="G1" s="65"/>
+    </row>
+    <row r="2" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="66"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="67"/>
+      <c r="G2" s="46"/>
+    </row>
+    <row r="3" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="68" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" s="69"/>
+      <c r="E3" s="69"/>
+      <c r="F3" s="69"/>
+      <c r="G3" s="70"/>
+    </row>
+    <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B4" s="57" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="46"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="59" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="60"/>
+      <c r="D5" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="61" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="60"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="14"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="59" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="60"/>
+      <c r="D7" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="16"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B8" s="62" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="60"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="18"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B9" s="59" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="60"/>
+      <c r="D9" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" s="19"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B10" s="48"/>
+      <c r="C10" s="49"/>
+      <c r="D10" s="49"/>
+      <c r="E10" s="49"/>
+      <c r="F10" s="49"/>
+      <c r="G10" s="50"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B11" s="51"/>
+      <c r="C11" s="52"/>
+      <c r="D11" s="52"/>
+      <c r="E11" s="52"/>
+      <c r="F11" s="52"/>
+      <c r="G11" s="53"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B12" s="51"/>
+      <c r="C12" s="52"/>
+      <c r="D12" s="52"/>
+      <c r="E12" s="52"/>
+      <c r="F12" s="52"/>
+      <c r="G12" s="53"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B13" s="54"/>
+      <c r="C13" s="55"/>
+      <c r="D13" s="55"/>
+      <c r="E13" s="55"/>
+      <c r="F13" s="55"/>
+      <c r="G13" s="56"/>
+    </row>
+    <row r="14" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B14" s="57" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="45"/>
+      <c r="D14" s="45"/>
+      <c r="E14" s="45"/>
+      <c r="F14" s="45"/>
+      <c r="G14" s="46"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B15" s="44" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" s="45"/>
+      <c r="D15" s="45"/>
+      <c r="E15" s="45"/>
+      <c r="F15" s="45"/>
+      <c r="G15" s="46"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B16" s="47" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="45"/>
+      <c r="D16" s="45"/>
+      <c r="E16" s="45"/>
+      <c r="F16" s="45"/>
+      <c r="G16" s="46"/>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17" s="47"/>
+      <c r="C17" s="45"/>
+      <c r="D17" s="45"/>
+      <c r="E17" s="45"/>
+      <c r="F17" s="45"/>
+      <c r="G17" s="46"/>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B18" s="58" t="s">
+        <v>31</v>
+      </c>
+      <c r="C18" s="45"/>
+      <c r="D18" s="45"/>
+      <c r="E18" s="45"/>
+      <c r="F18" s="45"/>
+      <c r="G18" s="46"/>
+    </row>
+    <row r="19" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B19" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="D19" s="30"/>
+      <c r="E19" s="30"/>
+      <c r="F19" s="30"/>
+      <c r="G19" s="31"/>
+    </row>
+    <row r="20" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="32"/>
+      <c r="C20" s="35"/>
+      <c r="D20" s="36"/>
+      <c r="E20" s="36"/>
+      <c r="F20" s="36"/>
+      <c r="G20" s="37"/>
+    </row>
+    <row r="21" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="33"/>
+      <c r="C21" s="38"/>
+      <c r="D21" s="39"/>
+      <c r="E21" s="39"/>
+      <c r="F21" s="39"/>
+      <c r="G21" s="40"/>
+    </row>
+    <row r="22" spans="2:7" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="33"/>
+      <c r="C22" s="38"/>
+      <c r="D22" s="39"/>
+      <c r="E22" s="39"/>
+      <c r="F22" s="39"/>
+      <c r="G22" s="40"/>
+    </row>
+    <row r="23" spans="2:7" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="33"/>
+      <c r="C23" s="38"/>
+      <c r="D23" s="39"/>
+      <c r="E23" s="39"/>
+      <c r="F23" s="39"/>
+      <c r="G23" s="40"/>
+    </row>
+    <row r="24" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="34"/>
+      <c r="C24" s="41"/>
+      <c r="D24" s="42"/>
+      <c r="E24" s="42"/>
+      <c r="F24" s="42"/>
+      <c r="G24" s="43"/>
+    </row>
+    <row r="25" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="44" t="s">
+        <v>34</v>
+      </c>
+      <c r="C25" s="45"/>
+      <c r="D25" s="45"/>
+      <c r="E25" s="45"/>
+      <c r="F25" s="45"/>
+      <c r="G25" s="46"/>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B26" s="47"/>
+      <c r="C26" s="45"/>
+      <c r="D26" s="45"/>
+      <c r="E26" s="45"/>
+      <c r="F26" s="45"/>
+      <c r="G26" s="46"/>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B27" s="47"/>
+      <c r="C27" s="45"/>
+      <c r="D27" s="45"/>
+      <c r="E27" s="45"/>
+      <c r="F27" s="45"/>
+      <c r="G27" s="46"/>
+    </row>
+  </sheetData>
+  <mergeCells count="22">
+    <mergeCell ref="C1:G1"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="B26:G26"/>
+    <mergeCell ref="B27:G27"/>
+    <mergeCell ref="B10:G13"/>
+    <mergeCell ref="B14:G14"/>
+    <mergeCell ref="B15:G15"/>
+    <mergeCell ref="B16:G16"/>
+    <mergeCell ref="B17:G17"/>
+    <mergeCell ref="B18:G18"/>
+    <mergeCell ref="C3:G3"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="B20:B24"/>
+    <mergeCell ref="C20:G24"/>
+    <mergeCell ref="B25:G25"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>